<commit_message>
Removed space after primary (education row) in "14. Estimation_Financial_Damage.xlsx"
</commit_message>
<xml_diff>
--- a/data/14. Estimation_Financial_Damage.xlsx
+++ b/data/14. Estimation_Financial_Damage.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/theophile_mt/Desktop/Work/Government of Vanuatu/Second documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/theophile_mt/Desktop/Work/Government of Vanuatu/vanuatu/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3C350E-1E4A-C44B-851F-37A81C8893D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B7C401A-A1FB-8E41-94BF-4AC296A9EA2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{D90494D9-DB17-D64C-B6B6-4EC777956C58}"/>
   </bookViews>
@@ -66,9 +66,6 @@
     <t>ecce</t>
   </si>
   <si>
-    <t>primary </t>
-  </si>
-  <si>
     <t>secondary</t>
   </si>
   <si>
@@ -253,6 +250,9 @@
   </si>
   <si>
     <t>Cluster</t>
+  </si>
+  <si>
+    <t>primary</t>
   </si>
 </sst>
 </file>
@@ -311,11 +311,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma [0] 2" xfId="2" xr:uid="{35A96A9B-6046-3145-923D-1D3B8191232A}"/>
@@ -638,7 +637,7 @@
   <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -650,20 +649,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>63</v>
+      <c r="E1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -694,7 +693,7 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>71</v>
       </c>
       <c r="E3" s="2">
         <v>5000000</v>
@@ -711,7 +710,7 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2">
         <v>10000000</v>
@@ -722,13 +721,13 @@
         <v>2025</v>
       </c>
       <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
       </c>
       <c r="E5" s="2">
         <v>100000000</v>
@@ -739,13 +738,13 @@
         <v>2025</v>
       </c>
       <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" s="2">
         <v>100000000</v>
@@ -756,13 +755,13 @@
         <v>2025</v>
       </c>
       <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
       </c>
       <c r="E7" s="2">
         <v>175000</v>
@@ -773,13 +772,13 @@
         <v>2025</v>
       </c>
       <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
         <v>15</v>
       </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
       <c r="D8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E8" s="2">
         <v>2500000</v>
@@ -790,13 +789,13 @@
         <v>2025</v>
       </c>
       <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
         <v>15</v>
       </c>
-      <c r="C9" t="s">
-        <v>16</v>
-      </c>
       <c r="D9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E9" s="2">
         <v>1000</v>
@@ -807,13 +806,13 @@
         <v>2025</v>
       </c>
       <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
         <v>15</v>
       </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
       <c r="D10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E10" s="2">
         <v>160000</v>
@@ -824,13 +823,13 @@
         <v>2025</v>
       </c>
       <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
         <v>18</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>19</v>
-      </c>
-      <c r="D11" t="s">
-        <v>20</v>
       </c>
       <c r="E11">
         <v>75</v>
@@ -841,13 +840,13 @@
         <v>2025</v>
       </c>
       <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
         <v>18</v>
       </c>
-      <c r="C12" t="s">
-        <v>19</v>
-      </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E12">
         <v>125</v>
@@ -858,13 +857,13 @@
         <v>2025</v>
       </c>
       <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
         <v>18</v>
       </c>
-      <c r="C13" t="s">
-        <v>19</v>
-      </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E13">
         <v>120</v>
@@ -875,13 +874,13 @@
         <v>2025</v>
       </c>
       <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
         <v>18</v>
       </c>
-      <c r="C14" t="s">
-        <v>19</v>
-      </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E14">
         <v>40</v>
@@ -892,13 +891,13 @@
         <v>2025</v>
       </c>
       <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
         <v>18</v>
       </c>
-      <c r="C15" t="s">
-        <v>19</v>
-      </c>
       <c r="D15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E15">
         <v>150</v>
@@ -909,13 +908,13 @@
         <v>2025</v>
       </c>
       <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
         <v>18</v>
       </c>
-      <c r="C16" t="s">
-        <v>19</v>
-      </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E16">
         <v>175</v>
@@ -926,13 +925,13 @@
         <v>2025</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" t="s">
         <v>26</v>
-      </c>
-      <c r="D17" t="s">
-        <v>27</v>
       </c>
       <c r="E17">
         <v>60</v>
@@ -943,13 +942,13 @@
         <v>2025</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E18">
         <v>120</v>
@@ -960,13 +959,13 @@
         <v>2025</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E19">
         <v>560</v>
@@ -977,13 +976,13 @@
         <v>2025</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E20">
         <v>1560</v>
@@ -994,13 +993,13 @@
         <v>2025</v>
       </c>
       <c r="B21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E21">
         <v>515</v>
@@ -1011,13 +1010,13 @@
         <v>2025</v>
       </c>
       <c r="B22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E22">
         <v>1200</v>
@@ -1028,13 +1027,13 @@
         <v>2025</v>
       </c>
       <c r="B23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E23">
         <v>225</v>
@@ -1045,13 +1044,13 @@
         <v>2025</v>
       </c>
       <c r="B24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E24">
         <v>10000</v>
@@ -1062,13 +1061,13 @@
         <v>2025</v>
       </c>
       <c r="B25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C25" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" t="s">
         <v>35</v>
-      </c>
-      <c r="D25" t="s">
-        <v>36</v>
       </c>
       <c r="E25" s="2">
         <v>70000</v>
@@ -1079,13 +1078,13 @@
         <v>2025</v>
       </c>
       <c r="B26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E26" s="2">
         <v>100000</v>
@@ -1096,13 +1095,13 @@
         <v>2025</v>
       </c>
       <c r="B27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E27" s="2">
         <v>80000</v>
@@ -1113,13 +1112,13 @@
         <v>2025</v>
       </c>
       <c r="B28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E28" s="2">
         <v>400000</v>
@@ -1130,13 +1129,13 @@
         <v>2025</v>
       </c>
       <c r="B29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E29" s="2">
         <v>300000</v>
@@ -1147,13 +1146,13 @@
         <v>2025</v>
       </c>
       <c r="B30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E30" s="2">
         <v>150000</v>
@@ -1164,13 +1163,13 @@
         <v>2025</v>
       </c>
       <c r="B31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E31" s="2">
         <v>600000</v>
@@ -1181,13 +1180,13 @@
         <v>2025</v>
       </c>
       <c r="B32" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" t="s">
         <v>43</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>44</v>
-      </c>
-      <c r="D32" t="s">
-        <v>45</v>
       </c>
       <c r="E32" s="2">
         <v>20000000</v>
@@ -1198,13 +1197,13 @@
         <v>2025</v>
       </c>
       <c r="B33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" t="s">
         <v>43</v>
       </c>
-      <c r="C33" t="s">
-        <v>44</v>
-      </c>
       <c r="D33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E33" s="2">
         <v>3000000</v>
@@ -1215,13 +1214,13 @@
         <v>2025</v>
       </c>
       <c r="B34" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" t="s">
         <v>43</v>
       </c>
-      <c r="C34" t="s">
-        <v>44</v>
-      </c>
       <c r="D34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E34">
         <v>5000000</v>
@@ -1232,13 +1231,13 @@
         <v>2025</v>
       </c>
       <c r="B35" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35" t="s">
         <v>43</v>
       </c>
-      <c r="C35" t="s">
-        <v>44</v>
-      </c>
       <c r="D35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E35" s="2">
         <v>12000000</v>
@@ -1252,10 +1251,10 @@
         <v>3</v>
       </c>
       <c r="C36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E36" s="2">
         <v>1000000</v>
@@ -1269,10 +1268,10 @@
         <v>3</v>
       </c>
       <c r="C37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E37" s="2">
         <v>500000</v>
@@ -1286,10 +1285,10 @@
         <v>3</v>
       </c>
       <c r="C38" t="s">
+        <v>49</v>
+      </c>
+      <c r="D38" t="s">
         <v>50</v>
-      </c>
-      <c r="D38" t="s">
-        <v>51</v>
       </c>
       <c r="E38" s="2">
         <v>1000000000</v>
@@ -1303,10 +1302,10 @@
         <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E39" s="2">
         <v>500000</v>
@@ -1320,10 +1319,10 @@
         <v>4</v>
       </c>
       <c r="C40" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D40" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E40" s="2">
         <v>15000000</v>
@@ -1337,10 +1336,10 @@
         <v>4</v>
       </c>
       <c r="C41" t="s">
+        <v>52</v>
+      </c>
+      <c r="D41" t="s">
         <v>53</v>
-      </c>
-      <c r="D41" t="s">
-        <v>54</v>
       </c>
       <c r="E41" s="2">
         <v>120000</v>
@@ -1354,10 +1353,10 @@
         <v>4</v>
       </c>
       <c r="C42" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E42" s="2">
         <v>130000</v>
@@ -1371,10 +1370,10 @@
         <v>5</v>
       </c>
       <c r="C43" t="s">
+        <v>55</v>
+      </c>
+      <c r="D43" t="s">
         <v>56</v>
-      </c>
-      <c r="D43" t="s">
-        <v>57</v>
       </c>
       <c r="E43" s="2">
         <v>200000</v>
@@ -1388,10 +1387,10 @@
         <v>5</v>
       </c>
       <c r="C44" t="s">
+        <v>57</v>
+      </c>
+      <c r="D44" t="s">
         <v>58</v>
-      </c>
-      <c r="D44" t="s">
-        <v>59</v>
       </c>
       <c r="E44" s="2">
         <v>400000</v>
@@ -1405,10 +1404,10 @@
         <v>5</v>
       </c>
       <c r="C45" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D45" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E45" s="2">
         <v>60000</v>
@@ -1422,10 +1421,10 @@
         <v>5</v>
       </c>
       <c r="C46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E46" s="2">
         <v>100000</v>
@@ -1439,10 +1438,10 @@
         <v>5</v>
       </c>
       <c r="C47" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D47" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E47" s="2">
         <v>200000</v>

</xml_diff>